<commit_message>
added function callback to update and render the data dynamically
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAX\OneDrive\Desktop\sem 4\python codes\BattleOFBytes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GALAX\OneDrive\Desktop\sem 4\python codes\BattleOFBytes\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB94E168-BCDC-45A8-A00F-13EF5F0EF879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE878F0-3019-4962-BA3B-466A0E90DAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{1CE4A62D-B6C7-4F22-90F0-23B73DD9D9EB}"/>
   </bookViews>
@@ -19,16 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -421,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D18200-9673-4B13-B03E-4E279E8CB5DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -535,16 +525,16 @@
         <v>700</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>